<commit_message>
Added quantities to products.
</commit_message>
<xml_diff>
--- a/Assets/MyShopDatasheet.xlsx
+++ b/Assets/MyShopDatasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANHQUANG\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANHQUANG\Desktop\StanData\Desktop\HCMUS\HK2-2122\WindowsProgramming\CodeRepo\WindowsProgramming_Project1\ShopManagementApp\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AF808D-954E-46F8-B537-FC051D05267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CBD054-CF81-4583-AEA3-49EEC9B269AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" activeTab="1" xr2:uid="{FB80D511-5DA5-4B11-B2D0-21ECE4A4677E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="106">
   <si>
     <t>Order</t>
   </si>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D983439-5BA4-451A-81AC-E7D5047C1CAE}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -784,7 +784,7 @@
     <col min="1" max="1" width="5.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.19921875" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.73046875" bestFit="1" customWidth="1"/>
   </cols>
@@ -822,6 +822,9 @@
       <c r="D2" s="1">
         <v>159</v>
       </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
       <c r="F2" t="s">
         <v>30</v>
       </c>
@@ -838,6 +841,9 @@
       </c>
       <c r="D3" s="1">
         <v>10.7</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -856,6 +862,9 @@
       <c r="D4" s="1">
         <v>61.99</v>
       </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -873,6 +882,9 @@
       <c r="D5" s="1">
         <v>13.99</v>
       </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
@@ -890,6 +902,9 @@
       <c r="D6" s="1">
         <v>11.39</v>
       </c>
+      <c r="E6">
+        <v>26</v>
+      </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
@@ -907,6 +922,9 @@
       <c r="D7" s="1">
         <v>9</v>
       </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
@@ -924,6 +942,9 @@
       <c r="D8" s="1">
         <v>59.99</v>
       </c>
+      <c r="E8">
+        <v>33</v>
+      </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
@@ -941,6 +962,9 @@
       <c r="D9" s="1">
         <v>102.64</v>
       </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
@@ -958,6 +982,9 @@
       <c r="D10" s="1">
         <v>48.99</v>
       </c>
+      <c r="E10">
+        <v>18</v>
+      </c>
       <c r="F10" t="s">
         <v>26</v>
       </c>
@@ -975,6 +1002,9 @@
       <c r="D11" s="1">
         <v>29.79</v>
       </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
       <c r="F11" t="s">
         <v>28</v>
       </c>
@@ -992,6 +1022,9 @@
       <c r="D12" s="1">
         <v>99</v>
       </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
       <c r="F12" t="s">
         <v>31</v>
       </c>
@@ -1009,6 +1042,9 @@
       <c r="D13" s="1">
         <v>17.87</v>
       </c>
+      <c r="E13">
+        <v>31</v>
+      </c>
       <c r="F13" t="s">
         <v>33</v>
       </c>
@@ -1026,6 +1062,9 @@
       <c r="D14" s="1">
         <v>16.37</v>
       </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
       <c r="F14" t="s">
         <v>35</v>
       </c>
@@ -1043,6 +1082,9 @@
       <c r="D15" s="1">
         <v>85</v>
       </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
       <c r="F15" t="s">
         <v>37</v>
       </c>
@@ -1060,6 +1102,9 @@
       <c r="D16" s="1">
         <v>8.9600000000000009</v>
       </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
       <c r="F16" t="s">
         <v>39</v>
       </c>
@@ -1077,6 +1122,9 @@
       <c r="D17" s="1">
         <v>6.67</v>
       </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
@@ -1094,6 +1142,9 @@
       <c r="D18" s="1">
         <v>89.99</v>
       </c>
+      <c r="E18">
+        <v>29</v>
+      </c>
       <c r="F18" t="s">
         <v>43</v>
       </c>
@@ -1111,6 +1162,9 @@
       <c r="D19" s="1">
         <v>34.5</v>
       </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
       <c r="F19" t="s">
         <v>46</v>
       </c>
@@ -1128,6 +1182,9 @@
       <c r="D20" s="1">
         <v>34.5</v>
       </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
       <c r="F20" t="s">
         <v>47</v>
       </c>
@@ -1145,6 +1202,9 @@
       <c r="D21" s="1">
         <v>15.39</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="F21" t="s">
         <v>49</v>
       </c>
@@ -1162,6 +1222,9 @@
       <c r="D22" s="1">
         <v>9.99</v>
       </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
       <c r="F22" t="s">
         <v>51</v>
       </c>
@@ -1179,6 +1242,9 @@
       <c r="D23" s="1">
         <v>99.99</v>
       </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
       <c r="F23" t="s">
         <v>53</v>
       </c>
@@ -1196,6 +1262,9 @@
       <c r="D24" s="1">
         <v>169</v>
       </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
       <c r="F24" t="s">
         <v>55</v>
       </c>
@@ -1213,6 +1282,9 @@
       <c r="D25" s="1">
         <v>99</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="F25" t="s">
         <v>57</v>
       </c>
@@ -1230,6 +1302,9 @@
       <c r="D26" s="1">
         <v>169</v>
       </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
       <c r="F26" t="s">
         <v>59</v>
       </c>
@@ -1247,6 +1322,9 @@
       <c r="D27" s="1">
         <v>16.079999999999998</v>
       </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
       <c r="F27" t="s">
         <v>61</v>
       </c>
@@ -1264,6 +1342,9 @@
       <c r="D28" s="1">
         <v>11.31</v>
       </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
       <c r="F28" t="s">
         <v>63</v>
       </c>
@@ -1281,6 +1362,9 @@
       <c r="D29" s="1">
         <v>56.99</v>
       </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
       <c r="F29" t="s">
         <v>65</v>
       </c>
@@ -1298,6 +1382,9 @@
       <c r="D30" s="1">
         <v>58</v>
       </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
       <c r="F30" t="s">
         <v>67</v>
       </c>
@@ -1315,6 +1402,9 @@
       <c r="D31" s="1">
         <v>479.49</v>
       </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
       <c r="F31" t="s">
         <v>69</v>
       </c>
@@ -1332,6 +1422,9 @@
       <c r="D32" s="1">
         <v>46.99</v>
       </c>
+      <c r="E32">
+        <v>21</v>
+      </c>
       <c r="F32" t="s">
         <v>71</v>
       </c>
@@ -1349,6 +1442,9 @@
       <c r="D33" s="1">
         <v>13.29</v>
       </c>
+      <c r="E33">
+        <v>9</v>
+      </c>
       <c r="F33" t="s">
         <v>73</v>
       </c>
@@ -1366,6 +1462,9 @@
       <c r="D34" s="1">
         <v>160.5</v>
       </c>
+      <c r="E34">
+        <v>23</v>
+      </c>
       <c r="F34" t="s">
         <v>75</v>
       </c>
@@ -1383,6 +1482,9 @@
       <c r="D35" s="1">
         <v>28.27</v>
       </c>
+      <c r="E35">
+        <v>21</v>
+      </c>
       <c r="F35" t="s">
         <v>77</v>
       </c>
@@ -1400,6 +1502,9 @@
       <c r="D36" s="1">
         <v>23.39</v>
       </c>
+      <c r="E36">
+        <v>9</v>
+      </c>
       <c r="F36" t="s">
         <v>79</v>
       </c>
@@ -1417,6 +1522,9 @@
       <c r="D37" s="1">
         <v>44.45</v>
       </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
       <c r="F37" t="s">
         <v>80</v>
       </c>
@@ -1434,6 +1542,9 @@
       <c r="D38" s="1">
         <v>13.76</v>
       </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
       <c r="F38" t="s">
         <v>83</v>
       </c>
@@ -1451,6 +1562,9 @@
       <c r="D39" s="1">
         <v>15.66</v>
       </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
       <c r="F39" t="s">
         <v>85</v>
       </c>
@@ -1468,6 +1582,9 @@
       <c r="D40" s="1">
         <v>18.97</v>
       </c>
+      <c r="E40">
+        <v>29</v>
+      </c>
       <c r="F40" t="s">
         <v>87</v>
       </c>
@@ -1485,6 +1602,9 @@
       <c r="D41" s="1">
         <v>19.61</v>
       </c>
+      <c r="E41">
+        <v>18</v>
+      </c>
       <c r="F41" t="s">
         <v>89</v>
       </c>
@@ -1502,6 +1622,9 @@
       <c r="D42" s="1">
         <v>14.36</v>
       </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
       <c r="F42" t="s">
         <v>91</v>
       </c>
@@ -1519,6 +1642,9 @@
       <c r="D43" s="1">
         <v>14.99</v>
       </c>
+      <c r="E43">
+        <v>28</v>
+      </c>
       <c r="F43" t="s">
         <v>93</v>
       </c>
@@ -1536,6 +1662,9 @@
       <c r="D44" s="1">
         <v>13.99</v>
       </c>
+      <c r="E44">
+        <v>12</v>
+      </c>
       <c r="F44" t="s">
         <v>95</v>
       </c>
@@ -1553,6 +1682,9 @@
       <c r="D45" s="1">
         <v>15.9</v>
       </c>
+      <c r="E45">
+        <v>14</v>
+      </c>
       <c r="F45" t="s">
         <v>97</v>
       </c>
@@ -1570,6 +1702,9 @@
       <c r="D46" s="1">
         <v>32.99</v>
       </c>
+      <c r="E46">
+        <v>16</v>
+      </c>
       <c r="F46" t="s">
         <v>98</v>
       </c>
@@ -1587,6 +1722,9 @@
       <c r="D47" s="1">
         <v>11.17</v>
       </c>
+      <c r="E47">
+        <v>32</v>
+      </c>
       <c r="F47" t="s">
         <v>101</v>
       </c>
@@ -1604,6 +1742,9 @@
       <c r="D48" s="1">
         <v>12.74</v>
       </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
       <c r="F48" t="s">
         <v>103</v>
       </c>
@@ -1620,6 +1761,9 @@
       </c>
       <c r="D49" s="1">
         <v>44.99</v>
+      </c>
+      <c r="E49">
+        <v>18</v>
       </c>
       <c r="F49" t="s">
         <v>105</v>

</xml_diff>